<commit_message>
first loop through 39 faculties
</commit_message>
<xml_diff>
--- a/PIList.xlsx
+++ b/PIList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/PIWordCloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A62E975E-8917-EC46-8A71-A18E9878CC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE08C0-C1D5-8E4F-AADA-DEF19A24F2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32480" yWindow="500" windowWidth="28280" windowHeight="25980" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
+    <workbookView xWindow="32480" yWindow="500" windowWidth="14620" windowHeight="19660" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Berrocal</t>
   </si>
@@ -113,6 +113,186 @@
   </si>
   <si>
     <t>Travis</t>
+  </si>
+  <si>
+    <t>New Faces</t>
+  </si>
+  <si>
+    <t>Allard</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Bogi</t>
+  </si>
+  <si>
+    <t>Beier</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Chesler</t>
+  </si>
+  <si>
+    <t>Naomi</t>
+  </si>
+  <si>
+    <t>Cho</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Enciso</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Ganesan</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Guindani</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>Kessenbrock</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>Lawson</t>
+  </si>
+  <si>
+    <t>Devon</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>Lowengrub</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Luo</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Marangoni</t>
+  </si>
+  <si>
+    <t>Francesco</t>
+  </si>
+  <si>
+    <t>Mortazavi</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Nie</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Schilling</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Seldin</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Shahbaba</t>
+  </si>
+  <si>
+    <t>Babak</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Swarup</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>Tsai</t>
+  </si>
+  <si>
+    <t>Sheryl</t>
+  </si>
+  <si>
+    <t>Xie</t>
+  </si>
+  <si>
+    <t>Xiaohui</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>Jing</t>
+  </si>
+  <si>
+    <t>Recent Intake</t>
+  </si>
+  <si>
+    <t>Anand</t>
+  </si>
+  <si>
+    <t>PI Last Name</t>
+  </si>
+  <si>
+    <t>PI First Name</t>
+  </si>
+  <si>
+    <t>PI Feature</t>
+  </si>
+  <si>
+    <t>Qing</t>
+  </si>
+  <si>
+    <t>New Faces, Recent Intake</t>
   </si>
 </sst>
 </file>
@@ -464,119 +644,474 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47278A47-5471-F54F-B299-7739D272D497}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B39" t="s">
         <v>25</v>
       </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
+    <sortCondition ref="A2:A41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commonness property to fix bug, old new faces
</commit_message>
<xml_diff>
--- a/PIList.xlsx
+++ b/PIList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/PIWordCloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9BFF3E-AD68-2D47-8291-099A324ED0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9BD9C0-7E61-C847-8C4D-B7A6AABE1A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="2000" windowWidth="28300" windowHeight="26060" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
+    <workbookView xWindow="48120" yWindow="1380" windowWidth="18720" windowHeight="21780" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="118">
   <si>
     <t>Berrocal</t>
   </si>
@@ -317,6 +317,78 @@
   </si>
   <si>
     <t>Andersen</t>
+  </si>
+  <si>
+    <t>Old New Faces</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>Wei</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Kvon</t>
+  </si>
+  <si>
+    <t>Evgeny</t>
+  </si>
+  <si>
+    <t>Shi</t>
+  </si>
+  <si>
+    <t>Xiaoyu</t>
+  </si>
+  <si>
+    <t>Yu</t>
+  </si>
+  <si>
+    <t>Jin</t>
+  </si>
+  <si>
+    <t>Rodriguez-Verdugo</t>
+  </si>
+  <si>
+    <t>Alejandra</t>
+  </si>
+  <si>
+    <t>Xu</t>
+  </si>
+  <si>
+    <t>Xiangmin</t>
+  </si>
+  <si>
+    <t>Marcu</t>
+  </si>
+  <si>
+    <t>Ding</t>
+  </si>
+  <si>
+    <t>Fanguayn</t>
+  </si>
+  <si>
+    <t>Siryaporn</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Komarova</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Wodarz</t>
+  </si>
+  <si>
+    <t>Dominik</t>
+  </si>
+  <si>
+    <t>Math bio</t>
   </si>
 </sst>
 </file>
@@ -668,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47278A47-5471-F54F-B299-7739D272D497}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,21 +876,21 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -826,10 +898,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -837,10 +909,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -848,10 +920,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
@@ -859,21 +931,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -881,21 +953,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
@@ -903,32 +975,32 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
         <v>75</v>
@@ -936,10 +1008,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>75</v>
@@ -947,54 +1019,54 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
         <v>75</v>
@@ -1002,10 +1074,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>75</v>
@@ -1013,87 +1085,87 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
         <v>75</v>
@@ -1101,65 +1173,65 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
         <v>75</v>
@@ -1167,18 +1239,150 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>73</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C57" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C47">
-    <sortCondition ref="A2:A47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
+    <sortCondition ref="A2:A58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vignettes with photos first 5 samples
</commit_message>
<xml_diff>
--- a/PIList.xlsx
+++ b/PIList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/PIWordCloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9BD9C0-7E61-C847-8C4D-B7A6AABE1A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F8CC57-CDAE-484D-9D40-0356CC24A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48120" yWindow="1380" windowWidth="18720" windowHeight="21780" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
   <si>
     <t>Berrocal</t>
   </si>
@@ -359,9 +359,6 @@
   </si>
   <si>
     <t>Xiangmin</t>
-  </si>
-  <si>
-    <t>Marcu</t>
   </si>
   <si>
     <t>Ding</t>
@@ -740,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47278A47-5471-F54F-B299-7739D272D497}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,10 +873,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
         <v>109</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>94</v>
@@ -975,13 +972,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
         <v>113</v>
       </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1220,18 +1217,18 @@
         <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
         <v>75</v>
@@ -1239,43 +1236,43 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
         <v>75</v>
@@ -1283,10 +1280,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
         <v>75</v>
@@ -1294,95 +1291,84 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
-    <sortCondition ref="A2:A58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C57">
+    <sortCondition ref="A2:A57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
begin modification to have mcsb logo
</commit_message>
<xml_diff>
--- a/PIList.xlsx
+++ b/PIList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/PIWordCloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060BD767-9FE9-E147-B4C9-973F32F9ECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D90298-FCD3-FF4B-8B03-3F63CAD86548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="500" windowWidth="19840" windowHeight="27360" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
+    <workbookView xWindow="1220" yWindow="11760" windowWidth="17660" windowHeight="16720" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,9 +424,6 @@
     <t>Medha</t>
   </si>
   <si>
-    <t>MCSB</t>
-  </si>
-  <si>
     <t>Kheradvar</t>
   </si>
   <si>
@@ -479,6 +476,9 @@
   </si>
   <si>
     <t>Wagar</t>
+  </si>
+  <si>
+    <t>isMCSB</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47278A47-5471-F54F-B299-7739D272D497}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +860,7 @@
         <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -879,6 +879,9 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -896,6 +899,9 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -913,6 +919,9 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -930,6 +939,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -945,6 +957,9 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
     </row>
@@ -964,6 +979,9 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -978,6 +996,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -995,6 +1016,9 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1012,6 +1036,9 @@
       <c r="E10">
         <v>0</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1029,6 +1056,9 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1046,6 +1076,9 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1060,6 +1093,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1077,6 +1113,9 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1091,6 +1130,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1108,8 +1150,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1125,8 +1170,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1142,8 +1190,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1159,8 +1210,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1176,8 +1230,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1193,8 +1250,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1210,8 +1270,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1227,8 +1290,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -1244,8 +1310,11 @@
       <c r="E24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1261,8 +1330,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1278,8 +1350,11 @@
       <c r="E26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1295,8 +1370,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1312,8 +1390,11 @@
       <c r="E28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1329,8 +1410,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1346,8 +1430,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -1363,8 +1450,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1380,8 +1470,11 @@
       <c r="E32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1397,8 +1490,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1414,8 +1510,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1431,8 +1530,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1448,8 +1550,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -1465,8 +1570,11 @@
       <c r="E37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -1482,8 +1590,11 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1499,8 +1610,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -1513,8 +1627,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1530,8 +1647,11 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -1547,8 +1667,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1564,8 +1687,11 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -1581,8 +1707,11 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1598,8 +1727,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -1615,8 +1747,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -1632,8 +1767,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1649,8 +1787,11 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -1666,8 +1807,11 @@
       <c r="E49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -1683,8 +1827,11 @@
       <c r="E50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -1700,8 +1847,11 @@
       <c r="E51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -1717,8 +1867,11 @@
       <c r="E52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -1734,8 +1887,11 @@
       <c r="E53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -1748,8 +1904,11 @@
       <c r="E54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -1765,8 +1924,11 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -1782,8 +1944,11 @@
       <c r="E56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -1799,8 +1964,11 @@
       <c r="E57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -1816,8 +1984,11 @@
       <c r="E58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -1833,8 +2004,11 @@
       <c r="E59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -1850,8 +2024,11 @@
       <c r="E60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -1867,157 +2044,187 @@
       <c r="E61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>130</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>138</v>
       </c>
-      <c r="C62" t="s">
-        <v>146</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="C63" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>131</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>139</v>
       </c>
-      <c r="C63" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="C64" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>132</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>140</v>
       </c>
-      <c r="C64" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="C65" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>133</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>141</v>
       </c>
-      <c r="C65" t="s">
-        <v>146</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="C66" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>134</v>
-      </c>
-      <c r="B66" t="s">
-        <v>142</v>
-      </c>
-      <c r="C66" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>135</v>
       </c>
       <c r="B67" t="s">
         <v>110</v>
       </c>
       <c r="C67" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" t="s">
+        <v>145</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>146</v>
       </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B69" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" t="s">
+        <v>145</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>136</v>
       </c>
-      <c r="B68" t="s">
-        <v>143</v>
-      </c>
-      <c r="C68" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>147</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>144</v>
       </c>
-      <c r="C69" t="s">
-        <v>146</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>145</v>
       </c>
-      <c r="C70" t="s">
-        <v>146</v>
-      </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first run with logo
</commit_message>
<xml_diff>
--- a/PIList.xlsx
+++ b/PIList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/PIWordCloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D90298-FCD3-FF4B-8B03-3F63CAD86548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED47B53C-65AE-E642-9508-827BE646EFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="11760" windowWidth="17660" windowHeight="16720" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
+    <workbookView xWindow="3460" yWindow="500" windowWidth="19720" windowHeight="25740" xr2:uid="{7EB06BE5-4E19-B849-8E68-317C10CC0817}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,13 +832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47278A47-5471-F54F-B299-7739D272D497}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
   </cols>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1965,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2145,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>